<commit_message>
CAmbios interfaz e indicadores
</commit_message>
<xml_diff>
--- a/src/Datos.xlsx
+++ b/src/Datos.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tec\Profesional\Semestre 7\sistema-Angeles\src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DA525D-D33F-469C-9D9E-099652F4979F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="EQUIPO" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="USUARIOS" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="MANTENIMIENTO" sheetId="3" r:id="rId6"/>
+    <sheet name="EQUIPO" sheetId="1" r:id="rId1"/>
+    <sheet name="USUARIOS" sheetId="2" r:id="rId2"/>
+    <sheet name="MANTENIMIENTO" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjxuRVN7ssEIGdSEeTFvCW5It1wBQ=="/>
@@ -18,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="213">
   <si>
     <t>Numero de control</t>
   </si>
@@ -654,39 +663,58 @@
   </si>
   <si>
     <t>AHER03388</t>
+  </si>
+  <si>
+    <t>.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -694,7 +722,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -722,7 +750,13 @@
     </fill>
   </fills>
   <borders count="12">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -730,27 +764,27 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -761,6 +795,18 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -771,176 +817,142 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="45">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1130,25 +1142,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="17" width="15.13"/>
-    <col customWidth="1" min="18" max="18" width="12.25"/>
-    <col customWidth="1" min="19" max="23" width="8.0"/>
+    <col min="1" max="17" width="15.125" customWidth="1"/>
+    <col min="18" max="18" width="12.25" customWidth="1"/>
+    <col min="19" max="23" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.75" customHeight="1">
+    <row r="1" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1221,7 @@
       <c r="V1" s="17"/>
       <c r="W1" s="17"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>42</v>
       </c>
@@ -1235,13 +1247,13 @@
         <v>53</v>
       </c>
       <c r="I2" s="19">
-        <v>154.0</v>
+        <v>154</v>
       </c>
       <c r="J2" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K2" s="19">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="L2" s="19" t="s">
         <v>59</v>
@@ -1262,10 +1274,10 @@
         <v>68</v>
       </c>
       <c r="R2" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>71</v>
       </c>
@@ -1291,13 +1303,13 @@
         <v>75</v>
       </c>
       <c r="I3" s="22">
-        <v>155.0</v>
+        <v>155</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K3" s="22">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="L3" s="22" t="s">
         <v>80</v>
@@ -1318,10 +1330,10 @@
         <v>88</v>
       </c>
       <c r="R3" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>89</v>
       </c>
@@ -1347,13 +1359,13 @@
         <v>91</v>
       </c>
       <c r="I4" s="19">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K4" s="19">
-        <v>2011.0</v>
+        <v>2011</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>59</v>
@@ -1371,10 +1383,10 @@
         <v>95</v>
       </c>
       <c r="R4" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>96</v>
       </c>
@@ -1400,13 +1412,13 @@
         <v>98</v>
       </c>
       <c r="I5" s="22">
-        <v>157.0</v>
+        <v>157</v>
       </c>
       <c r="J5" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K5" s="22">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="L5" s="22" t="s">
         <v>80</v>
@@ -1427,10 +1439,10 @@
         <v>100</v>
       </c>
       <c r="R5" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>101</v>
       </c>
@@ -1456,13 +1468,13 @@
         <v>53</v>
       </c>
       <c r="I6" s="19">
-        <v>158.0</v>
+        <v>158</v>
       </c>
       <c r="J6" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K6" s="19">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>59</v>
@@ -1480,10 +1492,10 @@
         <v>68</v>
       </c>
       <c r="R6" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>106</v>
       </c>
@@ -1509,13 +1521,13 @@
         <v>108</v>
       </c>
       <c r="I7" s="22">
-        <v>159.0</v>
+        <v>159</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K7" s="22">
-        <v>2008.0</v>
+        <v>2008</v>
       </c>
       <c r="L7" s="22" t="s">
         <v>80</v>
@@ -1536,10 +1548,10 @@
         <v>88</v>
       </c>
       <c r="R7" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>110</v>
       </c>
@@ -1565,13 +1577,13 @@
         <v>112</v>
       </c>
       <c r="I8" s="19">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="J8" s="22" t="s">
         <v>113</v>
       </c>
       <c r="K8" s="19">
-        <v>2007.0</v>
+        <v>2007</v>
       </c>
       <c r="L8" s="19" t="s">
         <v>59</v>
@@ -1589,10 +1601,10 @@
         <v>115</v>
       </c>
       <c r="R8" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>116</v>
       </c>
@@ -1616,13 +1628,13 @@
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="22">
-        <v>161.0</v>
+        <v>161</v>
       </c>
       <c r="J9" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K9" s="22">
-        <v>2006.0</v>
+        <v>2006</v>
       </c>
       <c r="L9" s="22" t="s">
         <v>80</v>
@@ -1643,10 +1655,10 @@
         <v>100</v>
       </c>
       <c r="R9" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>122</v>
       </c>
@@ -1672,13 +1684,13 @@
         <v>125</v>
       </c>
       <c r="I10" s="19">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="J10" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K10" s="19">
-        <v>2005.0</v>
+        <v>2005</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>59</v>
@@ -1699,10 +1711,10 @@
         <v>68</v>
       </c>
       <c r="R10" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>128</v>
       </c>
@@ -1728,13 +1740,13 @@
         <v>131</v>
       </c>
       <c r="I11" s="22">
-        <v>163.0</v>
+        <v>163</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K11" s="22">
-        <v>2004.0</v>
+        <v>2004</v>
       </c>
       <c r="L11" s="22" t="s">
         <v>80</v>
@@ -1755,10 +1767,10 @@
         <v>88</v>
       </c>
       <c r="R11" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>136</v>
       </c>
@@ -1784,13 +1796,13 @@
         <v>53</v>
       </c>
       <c r="I12" s="19">
-        <v>164.0</v>
+        <v>164</v>
       </c>
       <c r="J12" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K12" s="19">
-        <v>2003.0</v>
+        <v>2003</v>
       </c>
       <c r="L12" s="19" t="s">
         <v>59</v>
@@ -1808,10 +1820,10 @@
         <v>95</v>
       </c>
       <c r="R12" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>139</v>
       </c>
@@ -1837,13 +1849,13 @@
         <v>75</v>
       </c>
       <c r="I13" s="22">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="J13" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K13" s="22">
-        <v>2002.0</v>
+        <v>2002</v>
       </c>
       <c r="L13" s="22" t="s">
         <v>80</v>
@@ -1864,10 +1876,10 @@
         <v>100</v>
       </c>
       <c r="R13" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>141</v>
       </c>
@@ -1893,13 +1905,13 @@
         <v>91</v>
       </c>
       <c r="I14" s="19">
-        <v>166.0</v>
+        <v>166</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K14" s="19">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="L14" s="19" t="s">
         <v>59</v>
@@ -1917,10 +1929,10 @@
         <v>68</v>
       </c>
       <c r="R14" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>143</v>
       </c>
@@ -1946,13 +1958,13 @@
         <v>98</v>
       </c>
       <c r="I15" s="22">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="J15" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K15" s="22">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="L15" s="22" t="s">
         <v>80</v>
@@ -1973,10 +1985,10 @@
         <v>88</v>
       </c>
       <c r="R15" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>145</v>
       </c>
@@ -2002,13 +2014,13 @@
         <v>53</v>
       </c>
       <c r="I16" s="19">
-        <v>168.0</v>
+        <v>168</v>
       </c>
       <c r="J16" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K16" s="19">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>59</v>
@@ -2026,10 +2038,10 @@
         <v>115</v>
       </c>
       <c r="R16" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>147</v>
       </c>
@@ -2055,13 +2067,13 @@
         <v>108</v>
       </c>
       <c r="I17" s="22">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="J17" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K17" s="22">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="L17" s="22" t="s">
         <v>80</v>
@@ -2082,10 +2094,10 @@
         <v>100</v>
       </c>
       <c r="R17" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>149</v>
       </c>
@@ -2111,13 +2123,13 @@
         <v>112</v>
       </c>
       <c r="I18" s="19">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="J18" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K18" s="19">
-        <v>2011.0</v>
+        <v>2011</v>
       </c>
       <c r="L18" s="19" t="s">
         <v>59</v>
@@ -2138,10 +2150,10 @@
         <v>68</v>
       </c>
       <c r="R18" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>151</v>
       </c>
@@ -2165,13 +2177,13 @@
       </c>
       <c r="H19" s="25"/>
       <c r="I19" s="22">
-        <v>171.0</v>
+        <v>171</v>
       </c>
       <c r="J19" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K19" s="22">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>80</v>
@@ -2192,10 +2204,10 @@
         <v>88</v>
       </c>
       <c r="R19" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>154</v>
       </c>
@@ -2221,13 +2233,13 @@
         <v>125</v>
       </c>
       <c r="I20" s="19">
-        <v>172.0</v>
+        <v>172</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K20" s="19">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="L20" s="19" t="s">
         <v>59</v>
@@ -2245,10 +2257,10 @@
         <v>95</v>
       </c>
       <c r="R20" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>156</v>
       </c>
@@ -2274,13 +2286,13 @@
         <v>131</v>
       </c>
       <c r="I21" s="22">
-        <v>173.0</v>
+        <v>173</v>
       </c>
       <c r="J21" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K21" s="22">
-        <v>2008.0</v>
+        <v>2008</v>
       </c>
       <c r="L21" s="22" t="s">
         <v>80</v>
@@ -2301,10 +2313,10 @@
         <v>100</v>
       </c>
       <c r="R21" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>158</v>
       </c>
@@ -2328,13 +2340,13 @@
       </c>
       <c r="H22" s="25"/>
       <c r="I22" s="19">
-        <v>174.0</v>
+        <v>174</v>
       </c>
       <c r="J22" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K22" s="19">
-        <v>2007.0</v>
+        <v>2007</v>
       </c>
       <c r="L22" s="19" t="s">
         <v>59</v>
@@ -2352,10 +2364,10 @@
         <v>68</v>
       </c>
       <c r="R22" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>160</v>
       </c>
@@ -2381,13 +2393,13 @@
         <v>53</v>
       </c>
       <c r="I23" s="22">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K23" s="22">
-        <v>2006.0</v>
+        <v>2006</v>
       </c>
       <c r="L23" s="22" t="s">
         <v>80</v>
@@ -2408,10 +2420,10 @@
         <v>88</v>
       </c>
       <c r="R23" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>162</v>
       </c>
@@ -2437,13 +2449,13 @@
         <v>75</v>
       </c>
       <c r="I24" s="19">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="J24" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K24" s="19">
-        <v>2005.0</v>
+        <v>2005</v>
       </c>
       <c r="L24" s="19" t="s">
         <v>59</v>
@@ -2461,10 +2473,10 @@
         <v>115</v>
       </c>
       <c r="R24" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>164</v>
       </c>
@@ -2490,13 +2502,13 @@
         <v>91</v>
       </c>
       <c r="I25" s="22">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="J25" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K25" s="22">
-        <v>2004.0</v>
+        <v>2004</v>
       </c>
       <c r="L25" s="22" t="s">
         <v>80</v>
@@ -2517,10 +2529,10 @@
         <v>100</v>
       </c>
       <c r="R25" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>166</v>
       </c>
@@ -2546,13 +2558,13 @@
         <v>98</v>
       </c>
       <c r="I26" s="19">
-        <v>178.0</v>
+        <v>178</v>
       </c>
       <c r="J26" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K26" s="19">
-        <v>2003.0</v>
+        <v>2003</v>
       </c>
       <c r="L26" s="19" t="s">
         <v>59</v>
@@ -2573,10 +2585,10 @@
         <v>68</v>
       </c>
       <c r="R26" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>168</v>
       </c>
@@ -2602,13 +2614,13 @@
         <v>53</v>
       </c>
       <c r="I27" s="22">
-        <v>179.0</v>
+        <v>179</v>
       </c>
       <c r="J27" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K27" s="22">
-        <v>2002.0</v>
+        <v>2002</v>
       </c>
       <c r="L27" s="22" t="s">
         <v>80</v>
@@ -2629,10 +2641,10 @@
         <v>88</v>
       </c>
       <c r="R27" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>170</v>
       </c>
@@ -2658,13 +2670,13 @@
         <v>108</v>
       </c>
       <c r="I28" s="19">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="J28" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K28" s="19">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="L28" s="19" t="s">
         <v>59</v>
@@ -2682,10 +2694,10 @@
         <v>95</v>
       </c>
       <c r="R28" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>174</v>
       </c>
@@ -2711,13 +2723,13 @@
         <v>112</v>
       </c>
       <c r="I29" s="22">
-        <v>181.0</v>
+        <v>181</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K29" s="22">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="L29" s="22" t="s">
         <v>80</v>
@@ -2738,10 +2750,10 @@
         <v>100</v>
       </c>
       <c r="R29" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>175</v>
       </c>
@@ -2765,11 +2777,11 @@
       </c>
       <c r="H30" s="25"/>
       <c r="I30" s="19">
-        <v>182.0</v>
+        <v>182</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="19">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="L30" s="19" t="s">
         <v>59</v>
@@ -2787,10 +2799,10 @@
         <v>68</v>
       </c>
       <c r="R30" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>177</v>
       </c>
@@ -2804,7 +2816,7 @@
         <v>180</v>
       </c>
       <c r="E31" s="37">
-        <v>1.00907092423E11</v>
+        <v>100907092423</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>51</v>
@@ -2816,13 +2828,13 @@
         <v>125</v>
       </c>
       <c r="I31" s="22">
-        <v>183.0</v>
+        <v>183</v>
       </c>
       <c r="J31" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K31" s="22">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="L31" s="22" t="s">
         <v>80</v>
@@ -2843,10 +2855,10 @@
         <v>88</v>
       </c>
       <c r="R31" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>181</v>
       </c>
@@ -2860,7 +2872,7 @@
         <v>180</v>
       </c>
       <c r="E32" s="37">
-        <v>1.00907092424E11</v>
+        <v>100907092424</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>51</v>
@@ -2872,13 +2884,13 @@
         <v>131</v>
       </c>
       <c r="I32" s="19">
-        <v>184.0</v>
+        <v>184</v>
       </c>
       <c r="J32" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K32" s="19">
-        <v>2011.0</v>
+        <v>2011</v>
       </c>
       <c r="L32" s="19" t="s">
         <v>59</v>
@@ -2896,10 +2908,10 @@
         <v>115</v>
       </c>
       <c r="R32" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>182</v>
       </c>
@@ -2913,7 +2925,7 @@
         <v>180</v>
       </c>
       <c r="E33" s="37">
-        <v>1.00907092425E11</v>
+        <v>100907092425</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>51</v>
@@ -2925,13 +2937,13 @@
         <v>53</v>
       </c>
       <c r="I33" s="22">
-        <v>185.0</v>
+        <v>185</v>
       </c>
       <c r="J33" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K33" s="22">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="L33" s="22" t="s">
         <v>80</v>
@@ -2952,10 +2964,10 @@
         <v>100</v>
       </c>
       <c r="R33" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>183</v>
       </c>
@@ -2969,7 +2981,7 @@
         <v>180</v>
       </c>
       <c r="E34" s="37">
-        <v>1.00907092426E11</v>
+        <v>100907092426</v>
       </c>
       <c r="F34" s="19" t="s">
         <v>51</v>
@@ -2981,13 +2993,13 @@
         <v>75</v>
       </c>
       <c r="I34" s="19">
-        <v>186.0</v>
+        <v>186</v>
       </c>
       <c r="J34" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K34" s="19">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="L34" s="19" t="s">
         <v>59</v>
@@ -3008,10 +3020,10 @@
         <v>68</v>
       </c>
       <c r="R34" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>184</v>
       </c>
@@ -3025,7 +3037,7 @@
         <v>180</v>
       </c>
       <c r="E35" s="37">
-        <v>1.00907092427E11</v>
+        <v>100907092427</v>
       </c>
       <c r="F35" s="19" t="s">
         <v>51</v>
@@ -3037,13 +3049,13 @@
         <v>91</v>
       </c>
       <c r="I35" s="22">
-        <v>187.0</v>
+        <v>187</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K35" s="22">
-        <v>2008.0</v>
+        <v>2008</v>
       </c>
       <c r="L35" s="22" t="s">
         <v>80</v>
@@ -3064,10 +3076,10 @@
         <v>88</v>
       </c>
       <c r="R35" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>185</v>
       </c>
@@ -3081,7 +3093,7 @@
         <v>180</v>
       </c>
       <c r="E36" s="37">
-        <v>1.00907092428E11</v>
+        <v>100907092428</v>
       </c>
       <c r="F36" s="19" t="s">
         <v>51</v>
@@ -3093,13 +3105,13 @@
         <v>98</v>
       </c>
       <c r="I36" s="19">
-        <v>188.0</v>
+        <v>188</v>
       </c>
       <c r="J36" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K36" s="19">
-        <v>2007.0</v>
+        <v>2007</v>
       </c>
       <c r="L36" s="19" t="s">
         <v>59</v>
@@ -3117,10 +3129,10 @@
         <v>95</v>
       </c>
       <c r="R36" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>186</v>
       </c>
@@ -3134,7 +3146,7 @@
         <v>180</v>
       </c>
       <c r="E37" s="37">
-        <v>1.00907092429E11</v>
+        <v>100907092429</v>
       </c>
       <c r="F37" s="19" t="s">
         <v>51</v>
@@ -3146,13 +3158,13 @@
         <v>53</v>
       </c>
       <c r="I37" s="22">
-        <v>189.0</v>
+        <v>189</v>
       </c>
       <c r="J37" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K37" s="22">
-        <v>2006.0</v>
+        <v>2006</v>
       </c>
       <c r="L37" s="22" t="s">
         <v>80</v>
@@ -3173,10 +3185,10 @@
         <v>100</v>
       </c>
       <c r="R37" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>187</v>
       </c>
@@ -3202,13 +3214,13 @@
         <v>108</v>
       </c>
       <c r="I38" s="19">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="J38" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K38" s="19">
-        <v>2005.0</v>
+        <v>2005</v>
       </c>
       <c r="L38" s="19" t="s">
         <v>59</v>
@@ -3226,10 +3238,10 @@
         <v>68</v>
       </c>
       <c r="R38" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>189</v>
       </c>
@@ -3255,13 +3267,13 @@
         <v>112</v>
       </c>
       <c r="I39" s="22">
-        <v>191.0</v>
+        <v>191</v>
       </c>
       <c r="J39" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K39" s="22">
-        <v>2004.0</v>
+        <v>2004</v>
       </c>
       <c r="L39" s="22" t="s">
         <v>80</v>
@@ -3282,10 +3294,10 @@
         <v>88</v>
       </c>
       <c r="R39" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>190</v>
       </c>
@@ -3309,13 +3321,13 @@
       </c>
       <c r="H40" s="25"/>
       <c r="I40" s="19">
-        <v>192.0</v>
+        <v>192</v>
       </c>
       <c r="J40" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K40" s="19">
-        <v>2003.0</v>
+        <v>2003</v>
       </c>
       <c r="L40" s="19" t="s">
         <v>59</v>
@@ -3333,10 +3345,10 @@
         <v>115</v>
       </c>
       <c r="R40" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>193</v>
       </c>
@@ -3362,13 +3374,13 @@
         <v>125</v>
       </c>
       <c r="I41" s="22">
-        <v>193.0</v>
+        <v>193</v>
       </c>
       <c r="J41" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K41" s="22">
-        <v>2002.0</v>
+        <v>2002</v>
       </c>
       <c r="L41" s="22" t="s">
         <v>80</v>
@@ -3389,10 +3401,10 @@
         <v>100</v>
       </c>
       <c r="R41" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>46</v>
       </c>
@@ -3418,13 +3430,13 @@
         <v>131</v>
       </c>
       <c r="I42" s="19">
-        <v>194.0</v>
+        <v>194</v>
       </c>
       <c r="J42" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K42" s="19">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="L42" s="19" t="s">
         <v>59</v>
@@ -3445,10 +3457,10 @@
         <v>68</v>
       </c>
       <c r="R42" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>72</v>
       </c>
@@ -3472,13 +3484,13 @@
       </c>
       <c r="H43" s="25"/>
       <c r="I43" s="22">
-        <v>195.0</v>
+        <v>195</v>
       </c>
       <c r="J43" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K43" s="22">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="L43" s="22" t="s">
         <v>80</v>
@@ -3499,10 +3511,10 @@
         <v>88</v>
       </c>
       <c r="R43" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>99</v>
       </c>
@@ -3528,13 +3540,13 @@
         <v>53</v>
       </c>
       <c r="I44" s="19">
-        <v>196.0</v>
+        <v>196</v>
       </c>
       <c r="J44" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K44" s="19">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="L44" s="19" t="s">
         <v>59</v>
@@ -3552,10 +3564,10 @@
         <v>95</v>
       </c>
       <c r="R44" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>198</v>
       </c>
@@ -3581,13 +3593,13 @@
         <v>75</v>
       </c>
       <c r="I45" s="22">
-        <v>197.0</v>
+        <v>197</v>
       </c>
       <c r="J45" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K45" s="22">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="L45" s="22" t="s">
         <v>80</v>
@@ -3608,10 +3620,10 @@
         <v>100</v>
       </c>
       <c r="R45" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>199</v>
       </c>
@@ -3637,13 +3649,13 @@
         <v>91</v>
       </c>
       <c r="I46" s="19">
-        <v>198.0</v>
+        <v>198</v>
       </c>
       <c r="J46" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K46" s="19">
-        <v>2011.0</v>
+        <v>2011</v>
       </c>
       <c r="L46" s="19" t="s">
         <v>59</v>
@@ -3661,10 +3673,10 @@
         <v>68</v>
       </c>
       <c r="R46" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>200</v>
       </c>
@@ -3690,13 +3702,13 @@
         <v>98</v>
       </c>
       <c r="I47" s="22">
-        <v>199.0</v>
+        <v>199</v>
       </c>
       <c r="J47" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K47" s="22">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="L47" s="22" t="s">
         <v>80</v>
@@ -3717,10 +3729,10 @@
         <v>88</v>
       </c>
       <c r="R47" s="28">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>201</v>
       </c>
@@ -3746,13 +3758,13 @@
         <v>53</v>
       </c>
       <c r="I48" s="19">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="J48" s="22" t="s">
         <v>77</v>
       </c>
       <c r="K48" s="19">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="L48" s="19" t="s">
         <v>59</v>
@@ -3770,10 +3782,10 @@
         <v>115</v>
       </c>
       <c r="R48" s="28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>203</v>
       </c>
@@ -3799,13 +3811,13 @@
         <v>108</v>
       </c>
       <c r="I49" s="22">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="J49" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K49" s="22">
-        <v>2008.0</v>
+        <v>2008</v>
       </c>
       <c r="L49" s="22" t="s">
         <v>80</v>
@@ -3826,10 +3838,10 @@
         <v>100</v>
       </c>
       <c r="R49" s="28">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>206</v>
       </c>
@@ -3855,13 +3867,13 @@
         <v>112</v>
       </c>
       <c r="I50" s="19">
-        <v>202.0</v>
+        <v>202</v>
       </c>
       <c r="J50" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K50" s="19">
-        <v>2007.0</v>
+        <v>2007</v>
       </c>
       <c r="L50" s="19" t="s">
         <v>59</v>
@@ -3882,10 +3894,10 @@
         <v>53</v>
       </c>
       <c r="R50" s="28">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="38" t="s">
         <v>209</v>
       </c>
@@ -3909,13 +3921,13 @@
       </c>
       <c r="H51" s="41"/>
       <c r="I51" s="31">
-        <v>203.0</v>
+        <v>203</v>
       </c>
       <c r="J51" s="31" t="s">
         <v>77</v>
       </c>
       <c r="K51" s="31">
-        <v>2006.0</v>
+        <v>2006</v>
       </c>
       <c r="L51" s="31" t="s">
         <v>80</v>
@@ -3936,980 +3948,979 @@
         <v>112</v>
       </c>
       <c r="R51" s="36">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="18.25"/>
+    <col min="4" max="4" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4923,7 +4934,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>103</v>
       </c>
@@ -4934,10 +4945,10 @@
         <v>105</v>
       </c>
       <c r="D2" s="32">
-        <v>42370.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>119</v>
       </c>
@@ -4948,10 +4959,10 @@
         <v>121</v>
       </c>
       <c r="D3" s="32">
-        <v>42086.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>42086</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>124</v>
       </c>
@@ -4962,29 +4973,32 @@
         <v>105</v>
       </c>
       <c r="D4" s="34">
-        <v>38399.0</v>
+        <v>38399</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="8" max="8" width="17.63"/>
-    <col customWidth="1" min="23" max="23" width="14.13"/>
+    <col min="8" max="8" width="17.625" customWidth="1"/>
+    <col min="23" max="23" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -5055,9 +5069,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
-        <v>123.0</v>
+        <v>123</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>46</v>
@@ -5072,10 +5086,10 @@
         <v>49</v>
       </c>
       <c r="F2" s="24">
-        <v>43475.0</v>
+        <v>43475</v>
       </c>
       <c r="G2" s="24">
-        <v>43485.0</v>
+        <v>43485</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>51</v>
@@ -5086,26 +5100,26 @@
       <c r="J2" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="43" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="22" t="s">
         <v>57</v>
       </c>
       <c r="M2" s="22">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="N2" s="22">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="O2" s="26">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="P2" s="20">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="22">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="R2" s="22" t="s">
         <v>63</v>
@@ -5126,15 +5140,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
-        <v>124.0</v>
+        <v>124</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="22">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>48</v>
@@ -5143,10 +5157,10 @@
         <v>74</v>
       </c>
       <c r="F3" s="24">
-        <v>43480.0</v>
+        <v>43480</v>
       </c>
       <c r="G3" s="24">
-        <v>43490.0</v>
+        <v>43490</v>
       </c>
       <c r="H3" s="22" t="s">
         <v>51</v>
@@ -5164,19 +5178,19 @@
         <v>81</v>
       </c>
       <c r="M3" s="22">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="N3" s="22">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="O3" s="26">
-        <v>830.0</v>
+        <v>830</v>
       </c>
       <c r="P3" s="20">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="22">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="R3" s="22" t="s">
         <v>82</v>
@@ -5197,15 +5211,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="31">
-        <v>334.0</v>
+        <v>334</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>114</v>
@@ -5214,10 +5228,10 @@
         <v>49</v>
       </c>
       <c r="F4" s="33">
-        <v>43476.0</v>
+        <v>43476</v>
       </c>
       <c r="G4" s="33">
-        <v>43486.0</v>
+        <v>43486</v>
       </c>
       <c r="H4" s="31" t="s">
         <v>51</v>
@@ -5229,25 +5243,25 @@
         <v>126</v>
       </c>
       <c r="K4" s="31" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="L4" s="31" t="s">
         <v>127</v>
       </c>
       <c r="M4" s="31">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="N4" s="31">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="O4" s="35">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="P4" s="29" t="s">
         <v>130</v>
       </c>
       <c r="Q4" s="31">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="R4" s="31" t="s">
         <v>132</v>
@@ -5268,16 +5282,89 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6">
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
+        <v>126</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="31">
+        <v>335</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="33">
+        <v>43476</v>
+      </c>
+      <c r="G5" s="33">
+        <v>43486</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="K5" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="M5" s="31">
+        <v>200</v>
+      </c>
+      <c r="N5" s="31">
+        <v>100</v>
+      </c>
+      <c r="O5" s="35">
+        <v>350</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q5" s="31">
+        <v>101</v>
+      </c>
+      <c r="R5" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="S5" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="T5" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="U5" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="V5" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="W5" s="36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="W6" s="24"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="W7" s="24"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="W8" s="24"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>